<commit_message>
logging update in task
</commit_message>
<xml_diff>
--- a/data/raw_input_2_gener.xlsx
+++ b/data/raw_input_2_gener.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="902" uniqueCount="223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="902" uniqueCount="225">
   <si>
     <t xml:space="preserve">Date-time</t>
   </si>
@@ -115,6 +115,9 @@
     <t xml:space="preserve">A2%</t>
   </si>
   <si>
+    <t xml:space="preserve">A2p</t>
+  </si>
+  <si>
     <t xml:space="preserve">2022.02.28-12:21:53</t>
   </si>
   <si>
@@ -122,6 +125,9 @@
   </si>
   <si>
     <t xml:space="preserve">2022.02.28-12:31:15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A3p</t>
   </si>
   <si>
     <t xml:space="preserve">2022.02.28-14:00:00</t>
@@ -699,7 +705,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -728,13 +734,8 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
   </fonts>
-  <fills count="6">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -743,14 +744,38 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFDDDDDD"/>
+        <bgColor rgb="FFFFF5CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF729FCF"/>
+        <bgColor rgb="FF969696"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF5429"/>
+        <bgColor rgb="FFFF8080"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFB7B3CA"/>
-        <bgColor rgb="FFCCCCFF"/>
+        <bgColor rgb="FFAFD095"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFE994"/>
         <bgColor rgb="FFFFF5CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFAFD095"/>
+        <bgColor rgb="FFB7B3CA"/>
       </patternFill>
     </fill>
     <fill>
@@ -800,7 +825,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="15">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -809,15 +834,39 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -825,11 +874,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -860,14 +913,14 @@
       <rgbColor rgb="FF008080"/>
       <rgbColor rgb="FFB7B3CA"/>
       <rgbColor rgb="FF808080"/>
-      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF729FCF"/>
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FFFFF5CE"/>
       <rgbColor rgb="FFCCFFFF"/>
       <rgbColor rgb="FF660066"/>
       <rgbColor rgb="FFFF8080"/>
       <rgbColor rgb="FF0066CC"/>
-      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FFDDDDDD"/>
       <rgbColor rgb="FF000080"/>
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FFFFFF00"/>
@@ -880,7 +933,7 @@
       <rgbColor rgb="FFCCFFFF"/>
       <rgbColor rgb="FFCCFFCC"/>
       <rgbColor rgb="FFFFE994"/>
-      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFAFD095"/>
       <rgbColor rgb="FFFF99CC"/>
       <rgbColor rgb="FFCC99FF"/>
       <rgbColor rgb="FFFFCC99"/>
@@ -889,7 +942,7 @@
       <rgbColor rgb="FF99CC00"/>
       <rgbColor rgb="FFFFCC00"/>
       <rgbColor rgb="FFFF9900"/>
-      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FFFF5429"/>
       <rgbColor rgb="FF666699"/>
       <rgbColor rgb="FF969696"/>
       <rgbColor rgb="FF003366"/>
@@ -912,11 +965,11 @@
   </sheetPr>
   <dimension ref="A1:AG237"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="M1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AF1" activeCellId="0" sqref="AF:AF"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K24" activeCellId="0" sqref="K24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.96"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="15.61"/>
@@ -967,25 +1020,25 @@
       <c r="L2" s="0" t="s">
         <v>6</v>
       </c>
-      <c r="M2" s="0" t="n">
-        <v>10</v>
-      </c>
-      <c r="N2" s="0" t="n">
-        <v>10</v>
-      </c>
-      <c r="O2" s="0" t="n">
-        <v>10</v>
-      </c>
-      <c r="P2" s="0" t="n">
+      <c r="M2" s="2" t="n">
+        <v>10</v>
+      </c>
+      <c r="N2" s="2" t="n">
+        <v>10</v>
+      </c>
+      <c r="O2" s="2" t="n">
+        <v>10</v>
+      </c>
+      <c r="P2" s="2" t="n">
         <v>11</v>
       </c>
-      <c r="Q2" s="0" t="n">
+      <c r="Q2" s="2" t="n">
         <v>11</v>
       </c>
-      <c r="R2" s="0" t="n">
+      <c r="R2" s="2" t="n">
         <v>11</v>
       </c>
-      <c r="S2" s="0" t="n">
+      <c r="S2" s="2" t="n">
         <v>12</v>
       </c>
       <c r="T2" s="0" t="n">
@@ -1059,16 +1112,16 @@
       <c r="L3" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="M3" s="0" t="n">
+      <c r="M3" s="3" t="n">
         <v>-0.2</v>
       </c>
-      <c r="O3" s="1" t="n">
+      <c r="O3" s="4" t="n">
         <v>-0.2</v>
       </c>
-      <c r="P3" s="1" t="n">
+      <c r="P3" s="4" t="n">
         <v>-0.2</v>
       </c>
-      <c r="S3" s="1" t="n">
+      <c r="S3" s="4" t="n">
         <v>-0.2</v>
       </c>
       <c r="T3" s="1" t="n">
@@ -1127,13 +1180,13 @@
       <c r="L4" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="M4" s="0" t="n">
+      <c r="M4" s="5" t="n">
         <v>0.4</v>
       </c>
-      <c r="O4" s="0" t="n">
+      <c r="O4" s="5" t="n">
         <v>0.4</v>
       </c>
-      <c r="Q4" s="0" t="n">
+      <c r="Q4" s="5" t="n">
         <v>0.4</v>
       </c>
       <c r="T4" s="1" t="n">
@@ -1186,70 +1239,70 @@
       <c r="D6" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="K6" s="2" t="s">
+      <c r="K6" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="M6" s="3" t="s">
+      <c r="M6" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="N6" s="3" t="s">
+      <c r="N6" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="O6" s="3" t="s">
+      <c r="O6" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="P6" s="3" t="s">
+      <c r="P6" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="Q6" s="3" t="s">
+      <c r="Q6" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="R6" s="3" t="s">
+      <c r="R6" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="S6" s="3" t="s">
+      <c r="S6" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="T6" s="3" t="s">
+      <c r="T6" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="U6" s="3" t="s">
+      <c r="U6" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="V6" s="3" t="s">
+      <c r="V6" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="W6" s="3" t="s">
+      <c r="W6" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="X6" s="3" t="s">
+      <c r="X6" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="Y6" s="3" t="s">
+      <c r="Y6" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="Z6" s="3" t="s">
+      <c r="Z6" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="AA6" s="3" t="s">
+      <c r="AA6" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="AB6" s="3" t="s">
+      <c r="AB6" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="AC6" s="3" t="s">
+      <c r="AC6" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="AD6" s="3" t="s">
+      <c r="AD6" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="AE6" s="3" t="s">
+      <c r="AE6" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="AF6" s="3" t="s">
+      <c r="AF6" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="AG6" s="3" t="s">
+      <c r="AG6" s="7" t="s">
         <v>27</v>
       </c>
     </row>
@@ -1266,25 +1319,25 @@
       <c r="D7" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="M7" s="0" t="n">
+      <c r="M7" s="2" t="n">
         <v>0.6</v>
       </c>
-      <c r="N7" s="0" t="n">
+      <c r="N7" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="O7" s="0" t="n">
+      <c r="O7" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="P7" s="0" t="n">
+      <c r="P7" s="2" t="n">
         <v>0.8</v>
       </c>
-      <c r="Q7" s="0" t="n">
+      <c r="Q7" s="2" t="n">
         <v>0.7</v>
       </c>
-      <c r="R7" s="0" t="n">
+      <c r="R7" s="2" t="n">
         <v>0.5</v>
       </c>
-      <c r="S7" s="0" t="n">
+      <c r="S7" s="2" t="n">
         <v>0.5</v>
       </c>
       <c r="T7" s="0" t="n">
@@ -1343,19 +1396,19 @@
       <c r="D8" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="L8" s="0" t="s">
+      <c r="L8" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="M8" s="0" t="n">
+      <c r="M8" s="3" t="n">
         <v>0.2</v>
       </c>
-      <c r="O8" s="0" t="n">
+      <c r="O8" s="3" t="n">
         <v>0.6</v>
       </c>
-      <c r="P8" s="0" t="n">
+      <c r="P8" s="3" t="n">
         <v>0.5</v>
       </c>
-      <c r="S8" s="0" t="n">
+      <c r="S8" s="3" t="n">
         <v>0.9</v>
       </c>
       <c r="T8" s="0" t="n">
@@ -1397,33 +1450,33 @@
         <v>7</v>
       </c>
       <c r="L9" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="M9" s="0" t="n">
+        <v>31</v>
+      </c>
+      <c r="M9" s="9" t="n">
         <f aca="false">M$2*(1+(M3*M8))</f>
         <v>9.6</v>
       </c>
-      <c r="N9" s="0" t="n">
+      <c r="N9" s="9" t="n">
         <f aca="false">N$2*(1+(N3*N8))</f>
         <v>10</v>
       </c>
-      <c r="O9" s="0" t="n">
+      <c r="O9" s="9" t="n">
         <f aca="false">O$2*(1+(O3*O8))</f>
         <v>8.8</v>
       </c>
-      <c r="P9" s="0" t="n">
+      <c r="P9" s="9" t="n">
         <f aca="false">P$2*(1+(P3*P8))</f>
         <v>9.9</v>
       </c>
-      <c r="Q9" s="0" t="n">
+      <c r="Q9" s="9" t="n">
         <f aca="false">Q$2*(1+(Q3*Q8))</f>
         <v>11</v>
       </c>
-      <c r="R9" s="0" t="n">
+      <c r="R9" s="9" t="n">
         <f aca="false">R$2*(1+(R3*R8))</f>
         <v>11</v>
       </c>
-      <c r="S9" s="0" t="n">
+      <c r="S9" s="9" t="n">
         <f aca="false">S$2*(1+(S3*S8))</f>
         <v>9.84</v>
       </c>
@@ -1486,7 +1539,7 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>16</v>
@@ -1498,15 +1551,15 @@
         <v>10</v>
       </c>
       <c r="L10" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="M10" s="0" t="n">
+        <v>33</v>
+      </c>
+      <c r="M10" s="5" t="n">
         <v>0.7</v>
       </c>
-      <c r="O10" s="0" t="n">
+      <c r="O10" s="5" t="n">
         <v>0.5</v>
       </c>
-      <c r="Q10" s="0" t="n">
+      <c r="Q10" s="5" t="n">
         <v>0.3</v>
       </c>
       <c r="T10" s="0" t="n">
@@ -1530,7 +1583,7 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>5</v>
@@ -1542,33 +1595,33 @@
         <v>10</v>
       </c>
       <c r="L11" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="M11" s="0" t="n">
+        <v>35</v>
+      </c>
+      <c r="M11" s="9" t="n">
         <f aca="false">M$2*(1+(M4*M10))</f>
         <v>12.8</v>
       </c>
-      <c r="N11" s="0" t="n">
+      <c r="N11" s="9" t="n">
         <f aca="false">N$2*(1+(N4*N10))</f>
         <v>10</v>
       </c>
-      <c r="O11" s="0" t="n">
+      <c r="O11" s="9" t="n">
         <f aca="false">O$2*(1+(O4*O10))</f>
         <v>12</v>
       </c>
-      <c r="P11" s="0" t="n">
+      <c r="P11" s="9" t="n">
         <f aca="false">P$2*(1+(P4*P10))</f>
         <v>11</v>
       </c>
-      <c r="Q11" s="0" t="n">
+      <c r="Q11" s="9" t="n">
         <f aca="false">Q$2*(1+(Q4*Q10))</f>
         <v>12.32</v>
       </c>
-      <c r="R11" s="0" t="n">
+      <c r="R11" s="9" t="n">
         <f aca="false">R$2*(1+(R4*R10))</f>
         <v>11</v>
       </c>
-      <c r="S11" s="0" t="n">
+      <c r="S11" s="9" t="n">
         <f aca="false">S$2*(1+(S4*S10))</f>
         <v>12</v>
       </c>
@@ -1631,7 +1684,7 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>5</v>
@@ -1642,100 +1695,100 @@
       <c r="D12" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="K12" s="0" t="n">
+      <c r="K12" s="9" t="n">
         <v>0.2</v>
       </c>
-      <c r="L12" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="M12" s="3" t="n">
+      <c r="L12" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="M12" s="10" t="n">
         <f aca="false">M2*$K12*M7</f>
         <v>1.2</v>
       </c>
-      <c r="N12" s="3" t="n">
+      <c r="N12" s="10" t="n">
         <f aca="false">N2*$K12*N7</f>
         <v>2</v>
       </c>
-      <c r="O12" s="3" t="n">
+      <c r="O12" s="10" t="n">
         <f aca="false">O2*$K12*O7</f>
         <v>2</v>
       </c>
-      <c r="P12" s="3" t="n">
+      <c r="P12" s="10" t="n">
         <f aca="false">P2*$K12*P7</f>
         <v>1.76</v>
       </c>
-      <c r="Q12" s="3" t="n">
+      <c r="Q12" s="10" t="n">
         <f aca="false">Q2*$K12*Q7</f>
         <v>1.54</v>
       </c>
-      <c r="R12" s="3" t="n">
+      <c r="R12" s="10" t="n">
         <f aca="false">R2*$K12*R7</f>
         <v>1.1</v>
       </c>
-      <c r="S12" s="3" t="n">
+      <c r="S12" s="10" t="n">
         <f aca="false">S2*$K12*S7</f>
         <v>1.2</v>
       </c>
-      <c r="T12" s="3" t="n">
+      <c r="T12" s="7" t="n">
         <f aca="false">T2*$K12*T7</f>
         <v>1.44</v>
       </c>
-      <c r="U12" s="3" t="n">
+      <c r="U12" s="7" t="n">
         <f aca="false">U2*$K12*U7</f>
         <v>2.4</v>
       </c>
-      <c r="V12" s="3" t="n">
+      <c r="V12" s="7" t="n">
         <f aca="false">V2*$K12*V7</f>
         <v>2.6</v>
       </c>
-      <c r="W12" s="3" t="n">
+      <c r="W12" s="7" t="n">
         <f aca="false">W2*$K12*W7</f>
         <v>2.08</v>
       </c>
-      <c r="X12" s="3" t="n">
+      <c r="X12" s="7" t="n">
         <f aca="false">X2*$K12*X7</f>
         <v>1.82</v>
       </c>
-      <c r="Y12" s="3" t="n">
+      <c r="Y12" s="7" t="n">
         <f aca="false">Y2*$K12*Y7</f>
         <v>1.4</v>
       </c>
-      <c r="Z12" s="3" t="n">
+      <c r="Z12" s="7" t="n">
         <f aca="false">Z2*$K12*Z7</f>
         <v>1.4</v>
       </c>
-      <c r="AA12" s="3" t="n">
+      <c r="AA12" s="7" t="n">
         <f aca="false">AA2*$K12*AA7</f>
         <v>1.68</v>
       </c>
-      <c r="AB12" s="3" t="n">
+      <c r="AB12" s="7" t="n">
         <f aca="false">AB2*$K12*AB7</f>
         <v>3</v>
       </c>
-      <c r="AC12" s="3" t="n">
+      <c r="AC12" s="7" t="n">
         <f aca="false">AC2*$K12*AC7</f>
         <v>3</v>
       </c>
-      <c r="AD12" s="3" t="n">
+      <c r="AD12" s="7" t="n">
         <f aca="false">AD2*$K12*AD7</f>
         <v>2.4</v>
       </c>
-      <c r="AE12" s="3" t="n">
+      <c r="AE12" s="7" t="n">
         <f aca="false">AE2*$K12*AE7</f>
         <v>2.24</v>
       </c>
-      <c r="AF12" s="3" t="n">
+      <c r="AF12" s="7" t="n">
         <f aca="false">AF2*$K12*AF7</f>
         <v>1.6</v>
       </c>
-      <c r="AG12" s="3" t="n">
+      <c r="AG12" s="7" t="n">
         <f aca="false">AG2*$K12*AG7</f>
         <v>1.6</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>5</v>
@@ -1746,198 +1799,198 @@
       <c r="D13" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="J13" s="0" t="s">
+      <c r="J13" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="K13" s="0" t="n">
+      <c r="K13" s="9" t="n">
         <v>0.4</v>
       </c>
-      <c r="L13" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="M13" s="3" t="n">
+      <c r="L13" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="M13" s="4" t="n">
         <f aca="false">M9*$K13*M7</f>
         <v>2.304</v>
       </c>
-      <c r="N13" s="3" t="n">
+      <c r="N13" s="4" t="n">
         <f aca="false">N9*$K13*N7</f>
         <v>4</v>
       </c>
-      <c r="O13" s="3" t="n">
+      <c r="O13" s="4" t="n">
         <f aca="false">O9*$K13*O7</f>
         <v>3.52</v>
       </c>
-      <c r="P13" s="3" t="n">
+      <c r="P13" s="4" t="n">
         <f aca="false">P9*$K13*P7</f>
         <v>3.168</v>
       </c>
-      <c r="Q13" s="3" t="n">
+      <c r="Q13" s="4" t="n">
         <f aca="false">Q9*$K13*Q7</f>
         <v>3.08</v>
       </c>
-      <c r="R13" s="3" t="n">
+      <c r="R13" s="4" t="n">
         <f aca="false">R9*$K13*R7</f>
         <v>2.2</v>
       </c>
-      <c r="S13" s="3" t="n">
+      <c r="S13" s="4" t="n">
         <f aca="false">S9*$K13*S7</f>
         <v>1.968</v>
       </c>
-      <c r="T13" s="3" t="n">
+      <c r="T13" s="7" t="n">
         <f aca="false">T9*$K13*T7</f>
         <v>2.7648</v>
       </c>
-      <c r="U13" s="3" t="n">
+      <c r="U13" s="7" t="n">
         <f aca="false">U9*$K13*U7</f>
         <v>4.8</v>
       </c>
-      <c r="V13" s="3" t="n">
+      <c r="V13" s="7" t="n">
         <f aca="false">V9*$K13*V7</f>
         <v>4.576</v>
       </c>
-      <c r="W13" s="3" t="n">
+      <c r="W13" s="7" t="n">
         <f aca="false">W9*$K13*W7</f>
         <v>3.744</v>
       </c>
-      <c r="X13" s="3" t="n">
+      <c r="X13" s="7" t="n">
         <f aca="false">X9*$K13*X7</f>
         <v>3.64</v>
       </c>
-      <c r="Y13" s="3" t="n">
+      <c r="Y13" s="7" t="n">
         <f aca="false">Y9*$K13*Y7</f>
         <v>2.8</v>
       </c>
-      <c r="Z13" s="3" t="n">
+      <c r="Z13" s="7" t="n">
         <f aca="false">Z9*$K13*Z7</f>
         <v>2.296</v>
       </c>
-      <c r="AA13" s="3" t="n">
+      <c r="AA13" s="7" t="n">
         <f aca="false">AA9*$K13*AA7</f>
         <v>3.2256</v>
       </c>
-      <c r="AB13" s="3" t="n">
+      <c r="AB13" s="7" t="n">
         <f aca="false">AB9*$K13*AB7</f>
         <v>6</v>
       </c>
-      <c r="AC13" s="3" t="n">
+      <c r="AC13" s="7" t="n">
         <f aca="false">AC9*$K13*AC7</f>
         <v>5.28</v>
       </c>
-      <c r="AD13" s="3" t="n">
+      <c r="AD13" s="7" t="n">
         <f aca="false">AD9*$K13*AD7</f>
         <v>4.32</v>
       </c>
-      <c r="AE13" s="3" t="n">
+      <c r="AE13" s="7" t="n">
         <f aca="false">AE9*$K13*AE7</f>
         <v>4.48</v>
       </c>
-      <c r="AF13" s="3" t="n">
+      <c r="AF13" s="7" t="n">
         <f aca="false">AF9*$K13*AF7</f>
         <v>3.2</v>
       </c>
-      <c r="AG13" s="3" t="n">
+      <c r="AG13" s="7" t="n">
         <f aca="false">AG9*$K13*AG7</f>
         <v>2.624</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J14" s="0" t="s">
+      <c r="J14" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="K14" s="0" t="n">
+      <c r="K14" s="9" t="n">
         <v>0.25</v>
       </c>
-      <c r="L14" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="M14" s="3" t="n">
+      <c r="L14" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="M14" s="11" t="n">
         <f aca="false">M11*$K14*M7</f>
         <v>1.92</v>
       </c>
-      <c r="N14" s="3" t="n">
+      <c r="N14" s="11" t="n">
         <f aca="false">N11*$K14*N7</f>
         <v>2.5</v>
       </c>
-      <c r="O14" s="3" t="n">
+      <c r="O14" s="11" t="n">
         <f aca="false">O11*$K14*O7</f>
         <v>3</v>
       </c>
-      <c r="P14" s="3" t="n">
+      <c r="P14" s="11" t="n">
         <f aca="false">P11*$K14*P7</f>
         <v>2.2</v>
       </c>
-      <c r="Q14" s="3" t="n">
+      <c r="Q14" s="11" t="n">
         <f aca="false">Q11*$K14*Q7</f>
         <v>2.156</v>
       </c>
-      <c r="R14" s="3" t="n">
+      <c r="R14" s="11" t="n">
         <f aca="false">R11*$K14*R7</f>
         <v>1.375</v>
       </c>
-      <c r="S14" s="3" t="n">
+      <c r="S14" s="11" t="n">
         <f aca="false">S11*$K14*S7</f>
         <v>1.5</v>
       </c>
-      <c r="T14" s="3" t="n">
+      <c r="T14" s="7" t="n">
         <f aca="false">T11*$K14*T7</f>
         <v>2.304</v>
       </c>
-      <c r="U14" s="3" t="n">
+      <c r="U14" s="7" t="n">
         <f aca="false">U11*$K14*U7</f>
         <v>3</v>
       </c>
-      <c r="V14" s="3" t="n">
+      <c r="V14" s="7" t="n">
         <f aca="false">V11*$K14*V7</f>
         <v>3.9</v>
       </c>
-      <c r="W14" s="3" t="n">
+      <c r="W14" s="7" t="n">
         <f aca="false">W11*$K14*W7</f>
         <v>2.6</v>
       </c>
-      <c r="X14" s="3" t="n">
+      <c r="X14" s="7" t="n">
         <f aca="false">X11*$K14*X7</f>
         <v>2.548</v>
       </c>
-      <c r="Y14" s="3" t="n">
+      <c r="Y14" s="7" t="n">
         <f aca="false">Y11*$K14*Y7</f>
         <v>1.75</v>
       </c>
-      <c r="Z14" s="3" t="n">
+      <c r="Z14" s="7" t="n">
         <f aca="false">Z11*$K14*Z7</f>
         <v>1.75</v>
       </c>
-      <c r="AA14" s="3" t="n">
+      <c r="AA14" s="7" t="n">
         <f aca="false">AA11*$K14*AA7</f>
         <v>2.688</v>
       </c>
-      <c r="AB14" s="3" t="n">
+      <c r="AB14" s="7" t="n">
         <f aca="false">AB11*$K14*AB7</f>
         <v>3.75</v>
       </c>
-      <c r="AC14" s="3" t="n">
+      <c r="AC14" s="7" t="n">
         <f aca="false">AC11*$K14*AC7</f>
         <v>4.5</v>
       </c>
-      <c r="AD14" s="3" t="n">
+      <c r="AD14" s="7" t="n">
         <f aca="false">AD11*$K14*AD7</f>
         <v>3</v>
       </c>
-      <c r="AE14" s="3" t="n">
+      <c r="AE14" s="7" t="n">
         <f aca="false">AE11*$K14*AE7</f>
         <v>3.136</v>
       </c>
-      <c r="AF14" s="3" t="n">
+      <c r="AF14" s="7" t="n">
         <f aca="false">AF11*$K14*AF7</f>
         <v>2</v>
       </c>
-      <c r="AG14" s="3" t="n">
+      <c r="AG14" s="7" t="n">
         <f aca="false">AG11*$K14*AG7</f>
         <v>2</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>5</v>
@@ -1951,100 +2004,100 @@
       <c r="E15" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="K15" s="0" t="n">
+      <c r="K15" s="9" t="n">
         <v>0.15</v>
       </c>
-      <c r="L15" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="M15" s="3" t="n">
+      <c r="L15" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="M15" s="10" t="n">
         <f aca="false">$K15*M2*M7</f>
         <v>0.9</v>
       </c>
-      <c r="N15" s="3" t="n">
+      <c r="N15" s="10" t="n">
         <f aca="false">$K15*N2*N7</f>
         <v>1.5</v>
       </c>
-      <c r="O15" s="3" t="n">
+      <c r="O15" s="10" t="n">
         <f aca="false">$K15*O2*O7</f>
         <v>1.5</v>
       </c>
-      <c r="P15" s="3" t="n">
+      <c r="P15" s="10" t="n">
         <f aca="false">$K15*P2*P7</f>
         <v>1.32</v>
       </c>
-      <c r="Q15" s="3" t="n">
+      <c r="Q15" s="10" t="n">
         <f aca="false">$K15*Q2*Q7</f>
         <v>1.155</v>
       </c>
-      <c r="R15" s="3" t="n">
+      <c r="R15" s="10" t="n">
         <f aca="false">$K15*R2*R7</f>
         <v>0.825</v>
       </c>
-      <c r="S15" s="3" t="n">
+      <c r="S15" s="10" t="n">
         <f aca="false">$K15*S2*S7</f>
         <v>0.9</v>
       </c>
-      <c r="T15" s="3" t="n">
+      <c r="T15" s="7" t="n">
         <f aca="false">$K15*T2*T7</f>
         <v>1.08</v>
       </c>
-      <c r="U15" s="3" t="n">
+      <c r="U15" s="7" t="n">
         <f aca="false">$K15*U2*U7</f>
         <v>1.8</v>
       </c>
-      <c r="V15" s="3" t="n">
+      <c r="V15" s="7" t="n">
         <f aca="false">$K15*V2*V7</f>
         <v>1.95</v>
       </c>
-      <c r="W15" s="3" t="n">
+      <c r="W15" s="7" t="n">
         <f aca="false">$K15*W2*W7</f>
         <v>1.56</v>
       </c>
-      <c r="X15" s="3" t="n">
+      <c r="X15" s="7" t="n">
         <f aca="false">$K15*X2*X7</f>
         <v>1.365</v>
       </c>
-      <c r="Y15" s="3" t="n">
+      <c r="Y15" s="7" t="n">
         <f aca="false">$K15*Y2*Y7</f>
         <v>1.05</v>
       </c>
-      <c r="Z15" s="3" t="n">
+      <c r="Z15" s="7" t="n">
         <f aca="false">$K15*Z2*Z7</f>
         <v>1.05</v>
       </c>
-      <c r="AA15" s="3" t="n">
+      <c r="AA15" s="7" t="n">
         <f aca="false">$K15*AA2*AA7</f>
         <v>1.26</v>
       </c>
-      <c r="AB15" s="3" t="n">
+      <c r="AB15" s="7" t="n">
         <f aca="false">$K15*AB2*AB7</f>
         <v>2.25</v>
       </c>
-      <c r="AC15" s="3" t="n">
+      <c r="AC15" s="7" t="n">
         <f aca="false">$K15*AC2*AC7</f>
         <v>2.25</v>
       </c>
-      <c r="AD15" s="3" t="n">
+      <c r="AD15" s="7" t="n">
         <f aca="false">$K15*AD2*AD7</f>
         <v>1.8</v>
       </c>
-      <c r="AE15" s="3" t="n">
+      <c r="AE15" s="7" t="n">
         <f aca="false">$K15*AE2*AE7</f>
         <v>1.68</v>
       </c>
-      <c r="AF15" s="3" t="n">
+      <c r="AF15" s="7" t="n">
         <f aca="false">$K15*AF2*AF7</f>
         <v>1.2</v>
       </c>
-      <c r="AG15" s="3" t="n">
+      <c r="AG15" s="7" t="n">
         <f aca="false">$K15*AG2*AG7</f>
         <v>1.2</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>5</v>
@@ -2142,7 +2195,7 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>5</v>
@@ -2156,7 +2209,7 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>5</v>
@@ -2170,7 +2223,7 @@
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>5</v>
@@ -2184,7 +2237,7 @@
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>5</v>
@@ -2198,7 +2251,7 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>5</v>
@@ -2212,7 +2265,7 @@
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>5</v>
@@ -2223,13 +2276,13 @@
       <c r="D22" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="K22" s="2" t="s">
-        <v>48</v>
+      <c r="K22" s="6" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>5</v>
@@ -2333,7 +2386,7 @@
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>5</v>
@@ -2434,7 +2487,7 @@
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>5</v>
@@ -2535,7 +2588,7 @@
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>12</v>
@@ -2636,7 +2689,7 @@
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>12</v>
@@ -2650,7 +2703,7 @@
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>5</v>
@@ -2664,7 +2717,7 @@
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>5</v>
@@ -2675,13 +2728,13 @@
       <c r="D30" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="K30" s="2" t="s">
-        <v>55</v>
+      <c r="K30" s="6" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>16</v>
@@ -2695,7 +2748,7 @@
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>16</v>
@@ -2707,96 +2760,96 @@
         <v>10</v>
       </c>
       <c r="L32" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="M32" s="4" t="n">
+        <v>37</v>
+      </c>
+      <c r="M32" s="12" t="n">
         <f aca="false">ROUND(M24*3600,0)</f>
         <v>3000</v>
       </c>
-      <c r="N32" s="4" t="n">
+      <c r="N32" s="12" t="n">
         <f aca="false">ROUND(N24*3600,0)</f>
         <v>1800</v>
       </c>
-      <c r="O32" s="4" t="n">
+      <c r="O32" s="12" t="n">
         <f aca="false">ROUND(O24*3600,0)</f>
         <v>1800</v>
       </c>
-      <c r="P32" s="4" t="n">
+      <c r="P32" s="12" t="n">
         <f aca="false">ROUND(P24*3600,0)</f>
         <v>2045</v>
       </c>
-      <c r="Q32" s="4" t="n">
+      <c r="Q32" s="12" t="n">
         <f aca="false">ROUND(Q24*3600,0)</f>
         <v>2338</v>
       </c>
-      <c r="R32" s="4" t="n">
+      <c r="R32" s="12" t="n">
         <f aca="false">ROUND(R24*3600,0)</f>
         <v>3273</v>
       </c>
-      <c r="S32" s="4" t="n">
+      <c r="S32" s="12" t="n">
         <f aca="false">ROUND(S24*3600,0)</f>
         <v>3000</v>
       </c>
-      <c r="T32" s="4" t="n">
+      <c r="T32" s="12" t="n">
         <f aca="false">ROUND(T24*3600,0)</f>
         <v>2500</v>
       </c>
-      <c r="U32" s="4" t="n">
+      <c r="U32" s="12" t="n">
         <f aca="false">ROUND(U24*3600,0)</f>
         <v>1500</v>
       </c>
-      <c r="V32" s="4" t="n">
+      <c r="V32" s="12" t="n">
         <f aca="false">ROUND(V24*3600,0)</f>
         <v>1385</v>
       </c>
-      <c r="W32" s="4" t="n">
+      <c r="W32" s="12" t="n">
         <f aca="false">ROUND(W24*3600,0)</f>
         <v>1731</v>
       </c>
-      <c r="X32" s="4" t="n">
+      <c r="X32" s="12" t="n">
         <f aca="false">ROUND(X24*3600,0)</f>
         <v>1978</v>
       </c>
-      <c r="Y32" s="4" t="n">
+      <c r="Y32" s="12" t="n">
         <f aca="false">ROUND(Y24*3600,0)</f>
         <v>2571</v>
       </c>
-      <c r="Z32" s="4" t="n">
+      <c r="Z32" s="12" t="n">
         <f aca="false">ROUND(Z24*3600,0)</f>
         <v>2571</v>
       </c>
-      <c r="AA32" s="4" t="n">
+      <c r="AA32" s="12" t="n">
         <f aca="false">ROUND(AA24*3600,0)</f>
         <v>2143</v>
       </c>
-      <c r="AB32" s="4" t="n">
+      <c r="AB32" s="12" t="n">
         <f aca="false">ROUND(AB24*3600,0)</f>
         <v>1200</v>
       </c>
-      <c r="AC32" s="4" t="n">
+      <c r="AC32" s="12" t="n">
         <f aca="false">ROUND(AC24*3600,0)</f>
         <v>1200</v>
       </c>
-      <c r="AD32" s="4" t="n">
+      <c r="AD32" s="12" t="n">
         <f aca="false">ROUND(AD24*3600,0)</f>
         <v>1500</v>
       </c>
-      <c r="AE32" s="4" t="n">
+      <c r="AE32" s="12" t="n">
         <f aca="false">ROUND(AE24*3600,0)</f>
         <v>1607</v>
       </c>
-      <c r="AF32" s="4" t="n">
+      <c r="AF32" s="12" t="n">
         <f aca="false">ROUND(AF24*3600,0)</f>
         <v>2250</v>
       </c>
-      <c r="AG32" s="4" t="n">
+      <c r="AG32" s="12" t="n">
         <f aca="false">ROUND(AG24*3600,0)</f>
         <v>2250</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>5</v>
@@ -2808,96 +2861,96 @@
         <v>10</v>
       </c>
       <c r="L33" s="0" t="s">
-        <v>37</v>
-      </c>
-      <c r="M33" s="4" t="n">
+        <v>39</v>
+      </c>
+      <c r="M33" s="12" t="n">
         <f aca="false">ROUND(M25*3600,0)</f>
         <v>1563</v>
       </c>
-      <c r="N33" s="4" t="n">
+      <c r="N33" s="12" t="n">
         <f aca="false">ROUND(N25*3600,0)</f>
         <v>900</v>
       </c>
-      <c r="O33" s="4" t="n">
+      <c r="O33" s="12" t="n">
         <f aca="false">ROUND(O25*3600,0)</f>
         <v>1023</v>
       </c>
-      <c r="P33" s="4" t="n">
+      <c r="P33" s="12" t="n">
         <f aca="false">ROUND(P25*3600,0)</f>
         <v>1136</v>
       </c>
-      <c r="Q33" s="4" t="n">
+      <c r="Q33" s="12" t="n">
         <f aca="false">ROUND(Q25*3600,0)</f>
         <v>1169</v>
       </c>
-      <c r="R33" s="4" t="n">
+      <c r="R33" s="12" t="n">
         <f aca="false">ROUND(R25*3600,0)</f>
         <v>1636</v>
       </c>
-      <c r="S33" s="4" t="n">
+      <c r="S33" s="12" t="n">
         <f aca="false">ROUND(S25*3600,0)</f>
         <v>1829</v>
       </c>
-      <c r="T33" s="4" t="n">
+      <c r="T33" s="12" t="n">
         <f aca="false">ROUND(T25*3600,0)</f>
         <v>1302</v>
       </c>
-      <c r="U33" s="4" t="n">
+      <c r="U33" s="12" t="n">
         <f aca="false">ROUND(U25*3600,0)</f>
         <v>750</v>
       </c>
-      <c r="V33" s="4" t="n">
+      <c r="V33" s="12" t="n">
         <f aca="false">ROUND(V25*3600,0)</f>
         <v>787</v>
       </c>
-      <c r="W33" s="4" t="n">
+      <c r="W33" s="12" t="n">
         <f aca="false">ROUND(W25*3600,0)</f>
         <v>962</v>
       </c>
-      <c r="X33" s="4" t="n">
+      <c r="X33" s="12" t="n">
         <f aca="false">ROUND(X25*3600,0)</f>
         <v>989</v>
       </c>
-      <c r="Y33" s="4" t="n">
+      <c r="Y33" s="12" t="n">
         <f aca="false">ROUND(Y25*3600,0)</f>
         <v>1286</v>
       </c>
-      <c r="Z33" s="4" t="n">
+      <c r="Z33" s="12" t="n">
         <f aca="false">ROUND(Z25*3600,0)</f>
         <v>1568</v>
       </c>
-      <c r="AA33" s="4" t="n">
+      <c r="AA33" s="12" t="n">
         <f aca="false">ROUND(AA25*3600,0)</f>
         <v>1116</v>
       </c>
-      <c r="AB33" s="4" t="n">
+      <c r="AB33" s="12" t="n">
         <f aca="false">ROUND(AB25*3600,0)</f>
         <v>600</v>
       </c>
-      <c r="AC33" s="4" t="n">
+      <c r="AC33" s="12" t="n">
         <f aca="false">ROUND(AC25*3600,0)</f>
         <v>682</v>
       </c>
-      <c r="AD33" s="4" t="n">
+      <c r="AD33" s="12" t="n">
         <f aca="false">ROUND(AD25*3600,0)</f>
         <v>833</v>
       </c>
-      <c r="AE33" s="4" t="n">
+      <c r="AE33" s="12" t="n">
         <f aca="false">ROUND(AE25*3600,0)</f>
         <v>804</v>
       </c>
-      <c r="AF33" s="4" t="n">
+      <c r="AF33" s="12" t="n">
         <f aca="false">ROUND(AF25*3600,0)</f>
         <v>1125</v>
       </c>
-      <c r="AG33" s="4" t="n">
+      <c r="AG33" s="12" t="n">
         <f aca="false">ROUND(AG25*3600,0)</f>
         <v>1372</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>5</v>
@@ -2909,96 +2962,96 @@
         <v>7</v>
       </c>
       <c r="L34" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="M34" s="4" t="n">
+        <v>40</v>
+      </c>
+      <c r="M34" s="12" t="n">
         <f aca="false">ROUND(M26*3600,0)</f>
         <v>1875</v>
       </c>
-      <c r="N34" s="4" t="n">
+      <c r="N34" s="12" t="n">
         <f aca="false">ROUND(N26*3600,0)</f>
         <v>1440</v>
       </c>
-      <c r="O34" s="4" t="n">
+      <c r="O34" s="12" t="n">
         <f aca="false">ROUND(O26*3600,0)</f>
         <v>1200</v>
       </c>
-      <c r="P34" s="4" t="n">
+      <c r="P34" s="12" t="n">
         <f aca="false">ROUND(P26*3600,0)</f>
         <v>1636</v>
       </c>
-      <c r="Q34" s="4" t="n">
+      <c r="Q34" s="12" t="n">
         <f aca="false">ROUND(Q26*3600,0)</f>
         <v>1670</v>
       </c>
-      <c r="R34" s="4" t="n">
+      <c r="R34" s="12" t="n">
         <f aca="false">ROUND(R26*3600,0)</f>
         <v>2618</v>
       </c>
-      <c r="S34" s="4" t="n">
+      <c r="S34" s="12" t="n">
         <f aca="false">ROUND(S26*3600,0)</f>
         <v>2400</v>
       </c>
-      <c r="T34" s="4" t="n">
+      <c r="T34" s="12" t="n">
         <f aca="false">ROUND(T26*3600,0)</f>
         <v>1563</v>
       </c>
-      <c r="U34" s="4" t="n">
+      <c r="U34" s="12" t="n">
         <f aca="false">ROUND(U26*3600,0)</f>
         <v>1200</v>
       </c>
-      <c r="V34" s="4" t="n">
+      <c r="V34" s="12" t="n">
         <f aca="false">ROUND(V26*3600,0)</f>
         <v>923</v>
       </c>
-      <c r="W34" s="4" t="n">
+      <c r="W34" s="12" t="n">
         <f aca="false">ROUND(W26*3600,0)</f>
         <v>1385</v>
       </c>
-      <c r="X34" s="4" t="n">
+      <c r="X34" s="12" t="n">
         <f aca="false">ROUND(X26*3600,0)</f>
         <v>1413</v>
       </c>
-      <c r="Y34" s="4" t="n">
+      <c r="Y34" s="12" t="n">
         <f aca="false">ROUND(Y26*3600,0)</f>
         <v>2057</v>
       </c>
-      <c r="Z34" s="4" t="n">
+      <c r="Z34" s="12" t="n">
         <f aca="false">ROUND(Z26*3600,0)</f>
         <v>2057</v>
       </c>
-      <c r="AA34" s="4" t="n">
+      <c r="AA34" s="12" t="n">
         <f aca="false">ROUND(AA26*3600,0)</f>
         <v>1339</v>
       </c>
-      <c r="AB34" s="4" t="n">
+      <c r="AB34" s="12" t="n">
         <f aca="false">ROUND(AB26*3600,0)</f>
         <v>960</v>
       </c>
-      <c r="AC34" s="4" t="n">
+      <c r="AC34" s="12" t="n">
         <f aca="false">ROUND(AC26*3600,0)</f>
         <v>800</v>
       </c>
-      <c r="AD34" s="4" t="n">
+      <c r="AD34" s="12" t="n">
         <f aca="false">ROUND(AD26*3600,0)</f>
         <v>1200</v>
       </c>
-      <c r="AE34" s="4" t="n">
+      <c r="AE34" s="12" t="n">
         <f aca="false">ROUND(AE26*3600,0)</f>
         <v>1148</v>
       </c>
-      <c r="AF34" s="4" t="n">
+      <c r="AF34" s="12" t="n">
         <f aca="false">ROUND(AF26*3600,0)</f>
         <v>1800</v>
       </c>
-      <c r="AG34" s="4" t="n">
+      <c r="AG34" s="12" t="n">
         <f aca="false">ROUND(AG26*3600,0)</f>
         <v>1800</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>5</v>
@@ -3010,96 +3063,96 @@
         <v>10</v>
       </c>
       <c r="L35" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="M35" s="4" t="n">
+        <v>42</v>
+      </c>
+      <c r="M35" s="12" t="n">
         <f aca="false">ROUND(M27*3600,0)</f>
         <v>4000</v>
       </c>
-      <c r="N35" s="4" t="n">
+      <c r="N35" s="12" t="n">
         <f aca="false">ROUND(N27*3600,0)</f>
         <v>2400</v>
       </c>
-      <c r="O35" s="4" t="n">
+      <c r="O35" s="12" t="n">
         <f aca="false">ROUND(O27*3600,0)</f>
         <v>2400</v>
       </c>
-      <c r="P35" s="4" t="n">
+      <c r="P35" s="12" t="n">
         <f aca="false">ROUND(P27*3600,0)</f>
         <v>2727</v>
       </c>
-      <c r="Q35" s="4" t="n">
+      <c r="Q35" s="12" t="n">
         <f aca="false">ROUND(Q27*3600,0)</f>
         <v>3117</v>
       </c>
-      <c r="R35" s="4" t="n">
+      <c r="R35" s="12" t="n">
         <f aca="false">ROUND(R27*3600,0)</f>
         <v>4364</v>
       </c>
-      <c r="S35" s="4" t="n">
+      <c r="S35" s="12" t="n">
         <f aca="false">ROUND(S27*3600,0)</f>
         <v>4000</v>
       </c>
-      <c r="T35" s="4" t="n">
+      <c r="T35" s="12" t="n">
         <f aca="false">ROUND(T27*3600,0)</f>
         <v>3333</v>
       </c>
-      <c r="U35" s="4" t="n">
+      <c r="U35" s="12" t="n">
         <f aca="false">ROUND(U27*3600,0)</f>
         <v>2000</v>
       </c>
-      <c r="V35" s="4" t="n">
+      <c r="V35" s="12" t="n">
         <f aca="false">ROUND(V27*3600,0)</f>
         <v>1846</v>
       </c>
-      <c r="W35" s="4" t="n">
+      <c r="W35" s="12" t="n">
         <f aca="false">ROUND(W27*3600,0)</f>
         <v>2308</v>
       </c>
-      <c r="X35" s="4" t="n">
+      <c r="X35" s="12" t="n">
         <f aca="false">ROUND(X27*3600,0)</f>
         <v>2637</v>
       </c>
-      <c r="Y35" s="4" t="n">
+      <c r="Y35" s="12" t="n">
         <f aca="false">ROUND(Y27*3600,0)</f>
         <v>3429</v>
       </c>
-      <c r="Z35" s="4" t="n">
+      <c r="Z35" s="12" t="n">
         <f aca="false">ROUND(Z27*3600,0)</f>
         <v>3429</v>
       </c>
-      <c r="AA35" s="4" t="n">
+      <c r="AA35" s="12" t="n">
         <f aca="false">ROUND(AA27*3600,0)</f>
         <v>2857</v>
       </c>
-      <c r="AB35" s="4" t="n">
+      <c r="AB35" s="12" t="n">
         <f aca="false">ROUND(AB27*3600,0)</f>
         <v>1600</v>
       </c>
-      <c r="AC35" s="4" t="n">
+      <c r="AC35" s="12" t="n">
         <f aca="false">ROUND(AC27*3600,0)</f>
         <v>1600</v>
       </c>
-      <c r="AD35" s="4" t="n">
+      <c r="AD35" s="12" t="n">
         <f aca="false">ROUND(AD27*3600,0)</f>
         <v>2000</v>
       </c>
-      <c r="AE35" s="4" t="n">
+      <c r="AE35" s="12" t="n">
         <f aca="false">ROUND(AE27*3600,0)</f>
         <v>2143</v>
       </c>
-      <c r="AF35" s="4" t="n">
+      <c r="AF35" s="12" t="n">
         <f aca="false">ROUND(AF27*3600,0)</f>
         <v>3000</v>
       </c>
-      <c r="AG35" s="4" t="n">
+      <c r="AG35" s="12" t="n">
         <f aca="false">ROUND(AG27*3600,0)</f>
         <v>3000</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>5</v>
@@ -3113,13 +3166,13 @@
       <c r="E37" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="K37" s="2" t="s">
-        <v>61</v>
+      <c r="K37" s="6" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="1" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>5</v>
@@ -3133,7 +3186,7 @@
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B39" s="1" t="s">
         <v>5</v>
@@ -3148,96 +3201,96 @@
         <v>17</v>
       </c>
       <c r="L39" s="0" t="s">
-        <v>37</v>
-      </c>
-      <c r="M39" s="4" t="n">
+        <v>39</v>
+      </c>
+      <c r="M39" s="12" t="n">
         <f aca="false">ROUND(M33*M8,0)</f>
         <v>313</v>
       </c>
-      <c r="N39" s="4" t="n">
+      <c r="N39" s="12" t="n">
         <f aca="false">ROUND(N33*N8,0)</f>
         <v>0</v>
       </c>
-      <c r="O39" s="4" t="n">
+      <c r="O39" s="12" t="n">
         <f aca="false">ROUND(O33*O8,0)</f>
         <v>614</v>
       </c>
-      <c r="P39" s="4" t="n">
+      <c r="P39" s="12" t="n">
         <f aca="false">ROUND(P33*P8,0)</f>
         <v>568</v>
       </c>
-      <c r="Q39" s="4" t="n">
+      <c r="Q39" s="12" t="n">
         <f aca="false">ROUND(Q33*Q8,0)</f>
         <v>0</v>
       </c>
-      <c r="R39" s="4" t="n">
+      <c r="R39" s="12" t="n">
         <f aca="false">ROUND(R33*R8,0)</f>
         <v>0</v>
       </c>
-      <c r="S39" s="4" t="n">
+      <c r="S39" s="12" t="n">
         <f aca="false">ROUND(S33*S8,0)</f>
         <v>1646</v>
       </c>
-      <c r="T39" s="4" t="n">
+      <c r="T39" s="12" t="n">
         <f aca="false">ROUND(T33*T8,0)</f>
         <v>260</v>
       </c>
-      <c r="U39" s="4" t="n">
+      <c r="U39" s="12" t="n">
         <f aca="false">ROUND(U33*U8,0)</f>
         <v>0</v>
       </c>
-      <c r="V39" s="4" t="n">
+      <c r="V39" s="12" t="n">
         <f aca="false">ROUND(V33*V8,0)</f>
         <v>472</v>
       </c>
-      <c r="W39" s="4" t="n">
+      <c r="W39" s="12" t="n">
         <f aca="false">ROUND(W33*W8,0)</f>
         <v>481</v>
       </c>
-      <c r="X39" s="4" t="n">
+      <c r="X39" s="12" t="n">
         <f aca="false">ROUND(X33*X8,0)</f>
         <v>0</v>
       </c>
-      <c r="Y39" s="4" t="n">
+      <c r="Y39" s="12" t="n">
         <f aca="false">ROUND(Y33*Y8,0)</f>
         <v>0</v>
       </c>
-      <c r="Z39" s="4" t="n">
+      <c r="Z39" s="12" t="n">
         <f aca="false">ROUND(Z33*Z8,0)</f>
         <v>1411</v>
       </c>
-      <c r="AA39" s="5" t="n">
+      <c r="AA39" s="13" t="n">
         <f aca="false">ROUND(AA33*AA8,0)</f>
         <v>223</v>
       </c>
-      <c r="AB39" s="5" t="n">
+      <c r="AB39" s="13" t="n">
         <f aca="false">ROUND(AB33*AB8,0)</f>
         <v>0</v>
       </c>
-      <c r="AC39" s="5" t="n">
+      <c r="AC39" s="13" t="n">
         <f aca="false">ROUND(AC33*AC8,0)</f>
         <v>409</v>
       </c>
-      <c r="AD39" s="5" t="n">
+      <c r="AD39" s="13" t="n">
         <f aca="false">ROUND(AD33*AD8,0)</f>
         <v>417</v>
       </c>
-      <c r="AE39" s="5" t="n">
+      <c r="AE39" s="13" t="n">
         <f aca="false">ROUND(AE33*AE8,0)</f>
         <v>0</v>
       </c>
-      <c r="AF39" s="5" t="n">
+      <c r="AF39" s="13" t="n">
         <f aca="false">ROUND(AF33*AF8,0)</f>
         <v>0</v>
       </c>
-      <c r="AG39" s="5" t="n">
+      <c r="AG39" s="13" t="n">
         <f aca="false">ROUND(AG33*AG8,0)</f>
         <v>1235</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="1" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B40" s="1" t="s">
         <v>12</v>
@@ -3249,99 +3302,99 @@
         <v>7</v>
       </c>
       <c r="K40" s="0" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="L40" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="M40" s="4" t="n">
+        <v>40</v>
+      </c>
+      <c r="M40" s="12" t="n">
         <f aca="false">ROUND(M34*M10,0)</f>
         <v>1313</v>
       </c>
-      <c r="N40" s="4" t="n">
+      <c r="N40" s="12" t="n">
         <f aca="false">ROUND(N34*N10,0)</f>
         <v>0</v>
       </c>
-      <c r="O40" s="4" t="n">
+      <c r="O40" s="12" t="n">
         <f aca="false">ROUND(O34*O10,0)</f>
         <v>600</v>
       </c>
-      <c r="P40" s="4" t="n">
+      <c r="P40" s="12" t="n">
         <f aca="false">ROUND(P34*P10,0)</f>
         <v>0</v>
       </c>
-      <c r="Q40" s="4" t="n">
+      <c r="Q40" s="12" t="n">
         <f aca="false">ROUND(Q34*Q10,0)</f>
         <v>501</v>
       </c>
-      <c r="R40" s="4" t="n">
+      <c r="R40" s="12" t="n">
         <f aca="false">ROUND(R34*R10,0)</f>
         <v>0</v>
       </c>
-      <c r="S40" s="4" t="n">
+      <c r="S40" s="12" t="n">
         <f aca="false">ROUND(S34*S10,0)</f>
         <v>0</v>
       </c>
-      <c r="T40" s="4" t="n">
+      <c r="T40" s="12" t="n">
         <f aca="false">ROUND(T34*T10,0)</f>
         <v>1094</v>
       </c>
-      <c r="U40" s="4" t="n">
+      <c r="U40" s="12" t="n">
         <f aca="false">ROUND(U34*U10,0)</f>
         <v>0</v>
       </c>
-      <c r="V40" s="4" t="n">
+      <c r="V40" s="12" t="n">
         <f aca="false">ROUND(V34*V10,0)</f>
         <v>462</v>
       </c>
-      <c r="W40" s="4" t="n">
+      <c r="W40" s="12" t="n">
         <f aca="false">ROUND(W34*W10,0)</f>
         <v>0</v>
       </c>
-      <c r="X40" s="4" t="n">
+      <c r="X40" s="12" t="n">
         <f aca="false">ROUND(X34*X10,0)</f>
         <v>424</v>
       </c>
-      <c r="Y40" s="4" t="n">
+      <c r="Y40" s="12" t="n">
         <f aca="false">ROUND(Y34*Y10,0)</f>
         <v>0</v>
       </c>
-      <c r="Z40" s="4" t="n">
+      <c r="Z40" s="12" t="n">
         <f aca="false">ROUND(Z34*Z10,0)</f>
         <v>0</v>
       </c>
-      <c r="AA40" s="5" t="n">
+      <c r="AA40" s="13" t="n">
         <f aca="false">ROUND(AA34*AA10,0)</f>
         <v>937</v>
       </c>
-      <c r="AB40" s="5" t="n">
+      <c r="AB40" s="13" t="n">
         <f aca="false">ROUND(AB34*AB10,0)</f>
         <v>0</v>
       </c>
-      <c r="AC40" s="5" t="n">
+      <c r="AC40" s="13" t="n">
         <f aca="false">ROUND(AC34*AC10,0)</f>
         <v>400</v>
       </c>
-      <c r="AD40" s="5" t="n">
+      <c r="AD40" s="13" t="n">
         <f aca="false">ROUND(AD34*AD10,0)</f>
         <v>0</v>
       </c>
-      <c r="AE40" s="5" t="n">
+      <c r="AE40" s="13" t="n">
         <f aca="false">ROUND(AE34*AE10,0)</f>
         <v>344</v>
       </c>
-      <c r="AF40" s="5" t="n">
+      <c r="AF40" s="13" t="n">
         <f aca="false">ROUND(AF34*AF10,0)</f>
         <v>0</v>
       </c>
-      <c r="AG40" s="5" t="n">
+      <c r="AG40" s="13" t="n">
         <f aca="false">ROUND(AG34*AG10,0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="1" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>12</v>
@@ -3376,7 +3429,7 @@
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B42" s="1" t="s">
         <v>5</v>
@@ -3390,7 +3443,7 @@
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B43" s="1" t="s">
         <v>5</v>
@@ -3404,7 +3457,7 @@
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="1" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B44" s="1" t="s">
         <v>5</v>
@@ -3418,7 +3471,7 @@
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="B45" s="1" t="s">
         <v>5</v>
@@ -3432,7 +3485,7 @@
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="1" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="B46" s="1" t="s">
         <v>5</v>
@@ -3446,7 +3499,7 @@
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="B48" s="1" t="s">
         <v>5</v>
@@ -3463,7 +3516,7 @@
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="1" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="B49" s="1" t="s">
         <v>5</v>
@@ -3477,7 +3530,7 @@
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="1" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="B50" s="1" t="s">
         <v>5</v>
@@ -3491,7 +3544,7 @@
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="1" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="B51" s="1" t="s">
         <v>5</v>
@@ -3505,7 +3558,7 @@
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="1" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B52" s="1" t="s">
         <v>5</v>
@@ -3519,7 +3572,7 @@
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="1" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B53" s="1" t="s">
         <v>16</v>
@@ -3533,7 +3586,7 @@
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="1" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B54" s="1" t="s">
         <v>16</v>
@@ -3547,7 +3600,7 @@
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="1" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="B55" s="1" t="s">
         <v>5</v>
@@ -3561,7 +3614,7 @@
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="1" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="B56" s="1" t="s">
         <v>5</v>
@@ -3575,7 +3628,7 @@
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="1" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B57" s="1" t="s">
         <v>5</v>
@@ -3589,7 +3642,7 @@
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B59" s="1" t="s">
         <v>5</v>
@@ -3606,7 +3659,7 @@
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="1" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B60" s="1" t="s">
         <v>5</v>
@@ -3620,7 +3673,7 @@
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="1" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B61" s="1" t="s">
         <v>5</v>
@@ -3634,7 +3687,7 @@
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="1" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="B62" s="1" t="s">
         <v>5</v>
@@ -3648,7 +3701,7 @@
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="1" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="B63" s="1" t="s">
         <v>5</v>
@@ -3662,7 +3715,7 @@
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="1" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B64" s="1" t="s">
         <v>5</v>
@@ -3676,7 +3729,7 @@
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="1" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="B65" s="1" t="s">
         <v>5</v>
@@ -3690,7 +3743,7 @@
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="1" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="B66" s="1" t="s">
         <v>5</v>
@@ -3704,7 +3757,7 @@
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="1" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="B68" s="1" t="s">
         <v>5</v>
@@ -3721,7 +3774,7 @@
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="1" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="B69" s="1" t="s">
         <v>5</v>
@@ -3735,7 +3788,7 @@
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="1" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="B70" s="1" t="s">
         <v>5</v>
@@ -3749,7 +3802,7 @@
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="1" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="B71" s="1" t="s">
         <v>12</v>
@@ -3763,7 +3816,7 @@
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="1" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="B72" s="1" t="s">
         <v>12</v>
@@ -3777,7 +3830,7 @@
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="1" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="B73" s="1" t="s">
         <v>5</v>
@@ -3791,7 +3844,7 @@
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="0" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="B74" s="1" t="s">
         <v>5</v>
@@ -3805,7 +3858,7 @@
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="1" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="B75" s="1" t="s">
         <v>5</v>
@@ -3819,7 +3872,7 @@
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="1" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="B76" s="1" t="s">
         <v>5</v>
@@ -3833,7 +3886,7 @@
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="1" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="B77" s="1" t="s">
         <v>5</v>
@@ -3852,22 +3905,22 @@
       <c r="D78" s="1"/>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A79" s="6"/>
-      <c r="B79" s="6"/>
-      <c r="C79" s="6"/>
-      <c r="D79" s="6"/>
-      <c r="E79" s="6"/>
+      <c r="A79" s="14"/>
+      <c r="B79" s="14"/>
+      <c r="C79" s="14"/>
+      <c r="D79" s="14"/>
+      <c r="E79" s="14"/>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A80" s="6"/>
-      <c r="B80" s="6"/>
-      <c r="C80" s="6"/>
-      <c r="D80" s="6"/>
-      <c r="E80" s="6"/>
+      <c r="A80" s="14"/>
+      <c r="B80" s="14"/>
+      <c r="C80" s="14"/>
+      <c r="D80" s="14"/>
+      <c r="E80" s="14"/>
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="0" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="B82" s="1" t="s">
         <v>5</v>
@@ -3884,7 +3937,7 @@
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="1" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="B83" s="1" t="s">
         <v>5</v>
@@ -3898,7 +3951,7 @@
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="1" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="B84" s="1" t="s">
         <v>5</v>
@@ -3912,7 +3965,7 @@
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="1" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="B85" s="1" t="s">
         <v>12</v>
@@ -3926,7 +3979,7 @@
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="1" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="B86" s="1" t="s">
         <v>12</v>
@@ -3940,7 +3993,7 @@
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="1" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="B87" s="1" t="s">
         <v>5</v>
@@ -3954,7 +4007,7 @@
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="1" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="B88" s="1" t="s">
         <v>5</v>
@@ -3968,7 +4021,7 @@
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="1" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="B89" s="1" t="s">
         <v>16</v>
@@ -3982,7 +4035,7 @@
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="1" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="B90" s="1" t="s">
         <v>16</v>
@@ -3996,7 +4049,7 @@
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="1" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="B91" s="1" t="s">
         <v>5</v>
@@ -4010,7 +4063,7 @@
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="1" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="B92" s="1" t="s">
         <v>5</v>
@@ -4024,7 +4077,7 @@
     </row>
     <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="1" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="B93" s="1" t="s">
         <v>5</v>
@@ -4038,7 +4091,7 @@
     </row>
     <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="0" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="B95" s="1" t="s">
         <v>5</v>
@@ -4055,7 +4108,7 @@
     </row>
     <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="1" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="B96" s="1" t="s">
         <v>5</v>
@@ -4069,7 +4122,7 @@
     </row>
     <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="1" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="B97" s="1" t="s">
         <v>5</v>
@@ -4083,7 +4136,7 @@
     </row>
     <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="1" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="B98" s="1" t="s">
         <v>5</v>
@@ -4097,7 +4150,7 @@
     </row>
     <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="1" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="B99" s="1" t="s">
         <v>5</v>
@@ -4111,7 +4164,7 @@
     </row>
     <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="1" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="B100" s="1" t="s">
         <v>5</v>
@@ -4125,7 +4178,7 @@
     </row>
     <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="1" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="B101" s="1" t="s">
         <v>5</v>
@@ -4139,7 +4192,7 @@
     </row>
     <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="1" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="B102" s="1" t="s">
         <v>5</v>
@@ -4153,7 +4206,7 @@
     </row>
     <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="1" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="B104" s="1" t="s">
         <v>5</v>
@@ -4170,7 +4223,7 @@
     </row>
     <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="1" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="B105" s="1" t="s">
         <v>5</v>
@@ -4184,7 +4237,7 @@
     </row>
     <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="1" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="B106" s="1" t="s">
         <v>5</v>
@@ -4198,7 +4251,7 @@
     </row>
     <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="1" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="B107" s="1" t="s">
         <v>12</v>
@@ -4212,7 +4265,7 @@
     </row>
     <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="1" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="B108" s="1" t="s">
         <v>12</v>
@@ -4226,7 +4279,7 @@
     </row>
     <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="1" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="B109" s="1" t="s">
         <v>5</v>
@@ -4240,7 +4293,7 @@
     </row>
     <row r="110" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="0" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="B110" s="1" t="s">
         <v>5</v>
@@ -4254,7 +4307,7 @@
     </row>
     <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="1" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="B111" s="1" t="s">
         <v>16</v>
@@ -4268,7 +4321,7 @@
     </row>
     <row r="112" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="1" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="B112" s="1" t="s">
         <v>16</v>
@@ -4282,7 +4335,7 @@
     </row>
     <row r="113" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="1" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="B113" s="1" t="s">
         <v>5</v>
@@ -4296,7 +4349,7 @@
     </row>
     <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="1" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="B114" s="1" t="s">
         <v>5</v>
@@ -4310,7 +4363,7 @@
     </row>
     <row r="115" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="1" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="B115" s="1" t="s">
         <v>5</v>
@@ -4324,7 +4377,7 @@
     </row>
     <row r="117" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="1" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="B117" s="1" t="s">
         <v>5</v>
@@ -4341,7 +4394,7 @@
     </row>
     <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="1" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="B118" s="1" t="s">
         <v>5</v>
@@ -4355,7 +4408,7 @@
     </row>
     <row r="119" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="1" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="B119" s="1" t="s">
         <v>5</v>
@@ -4369,7 +4422,7 @@
     </row>
     <row r="120" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="1" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="B120" s="1" t="s">
         <v>12</v>
@@ -4383,7 +4436,7 @@
     </row>
     <row r="121" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="1" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="B121" s="1" t="s">
         <v>12</v>
@@ -4397,7 +4450,7 @@
     </row>
     <row r="122" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="1" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="B122" s="1" t="s">
         <v>5</v>
@@ -4411,7 +4464,7 @@
     </row>
     <row r="123" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="0" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="B123" s="1" t="s">
         <v>5</v>
@@ -4425,7 +4478,7 @@
     </row>
     <row r="124" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="1" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="B124" s="1" t="s">
         <v>5</v>
@@ -4439,7 +4492,7 @@
     </row>
     <row r="125" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="1" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="B125" s="1" t="s">
         <v>5</v>
@@ -4453,7 +4506,7 @@
     </row>
     <row r="126" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A126" s="1" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="B126" s="1" t="s">
         <v>5</v>
@@ -4467,7 +4520,7 @@
     </row>
     <row r="128" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A128" s="0" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="B128" s="1" t="s">
         <v>5</v>
@@ -4484,7 +4537,7 @@
     </row>
     <row r="129" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A129" s="1" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="B129" s="1" t="s">
         <v>5</v>
@@ -4498,7 +4551,7 @@
     </row>
     <row r="130" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="1" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="B130" s="1" t="s">
         <v>5</v>
@@ -4512,7 +4565,7 @@
     </row>
     <row r="131" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A131" s="1" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="B131" s="1" t="s">
         <v>5</v>
@@ -4526,7 +4579,7 @@
     </row>
     <row r="132" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A132" s="1" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="B132" s="1" t="s">
         <v>5</v>
@@ -4540,7 +4593,7 @@
     </row>
     <row r="133" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A133" s="1" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="B133" s="1" t="s">
         <v>16</v>
@@ -4554,7 +4607,7 @@
     </row>
     <row r="134" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="1" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="B134" s="1" t="s">
         <v>16</v>
@@ -4568,7 +4621,7 @@
     </row>
     <row r="135" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A135" s="1" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="B135" s="1" t="s">
         <v>5</v>
@@ -4582,7 +4635,7 @@
     </row>
     <row r="136" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A136" s="1" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="B136" s="1" t="s">
         <v>5</v>
@@ -4596,7 +4649,7 @@
     </row>
     <row r="137" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A137" s="1" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="B137" s="1" t="s">
         <v>5</v>
@@ -4610,7 +4663,7 @@
     </row>
     <row r="139" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A139" s="0" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="B139" s="1" t="s">
         <v>5</v>
@@ -4627,7 +4680,7 @@
     </row>
     <row r="140" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A140" s="1" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="B140" s="1" t="s">
         <v>5</v>
@@ -4641,7 +4694,7 @@
     </row>
     <row r="141" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A141" s="1" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="B141" s="1" t="s">
         <v>5</v>
@@ -4655,7 +4708,7 @@
     </row>
     <row r="142" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A142" s="1" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="B142" s="1" t="s">
         <v>5</v>
@@ -4669,7 +4722,7 @@
     </row>
     <row r="143" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A143" s="1" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="B143" s="1" t="s">
         <v>5</v>
@@ -4683,7 +4736,7 @@
     </row>
     <row r="144" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A144" s="1" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="B144" s="1" t="s">
         <v>5</v>
@@ -4697,7 +4750,7 @@
     </row>
     <row r="145" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A145" s="1" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="B145" s="1" t="s">
         <v>5</v>
@@ -4711,7 +4764,7 @@
     </row>
     <row r="146" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A146" s="1" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="B146" s="1" t="s">
         <v>5</v>
@@ -4725,7 +4778,7 @@
     </row>
     <row r="148" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A148" s="1" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="B148" s="1" t="s">
         <v>5</v>
@@ -4742,7 +4795,7 @@
     </row>
     <row r="149" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A149" s="1" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="B149" s="1" t="s">
         <v>5</v>
@@ -4756,7 +4809,7 @@
     </row>
     <row r="150" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A150" s="1" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="B150" s="1" t="s">
         <v>5</v>
@@ -4770,7 +4823,7 @@
     </row>
     <row r="151" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A151" s="1" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="B151" s="1" t="s">
         <v>12</v>
@@ -4784,7 +4837,7 @@
     </row>
     <row r="152" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A152" s="1" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="B152" s="1" t="s">
         <v>12</v>
@@ -4798,7 +4851,7 @@
     </row>
     <row r="153" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A153" s="1" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="B153" s="1" t="s">
         <v>5</v>
@@ -4812,7 +4865,7 @@
     </row>
     <row r="154" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A154" s="0" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="B154" s="1" t="s">
         <v>5</v>
@@ -4826,7 +4879,7 @@
     </row>
     <row r="155" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A155" s="1" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="B155" s="1" t="s">
         <v>5</v>
@@ -4840,7 +4893,7 @@
     </row>
     <row r="156" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A156" s="1" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="B156" s="1" t="s">
         <v>5</v>
@@ -4854,7 +4907,7 @@
     </row>
     <row r="157" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A157" s="1" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="B157" s="1" t="s">
         <v>5</v>
@@ -4867,22 +4920,22 @@
       </c>
     </row>
     <row r="159" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A159" s="6"/>
-      <c r="B159" s="6"/>
-      <c r="C159" s="6"/>
-      <c r="D159" s="6"/>
-      <c r="E159" s="6"/>
+      <c r="A159" s="14"/>
+      <c r="B159" s="14"/>
+      <c r="C159" s="14"/>
+      <c r="D159" s="14"/>
+      <c r="E159" s="14"/>
     </row>
     <row r="160" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A160" s="6"/>
-      <c r="B160" s="6"/>
-      <c r="C160" s="6"/>
-      <c r="D160" s="6"/>
-      <c r="E160" s="6"/>
+      <c r="A160" s="14"/>
+      <c r="B160" s="14"/>
+      <c r="C160" s="14"/>
+      <c r="D160" s="14"/>
+      <c r="E160" s="14"/>
     </row>
     <row r="162" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A162" s="0" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="B162" s="1" t="s">
         <v>5</v>
@@ -4898,8 +4951,8 @@
       </c>
     </row>
     <row r="163" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A163" s="7" t="s">
-        <v>161</v>
+      <c r="A163" s="1" t="s">
+        <v>163</v>
       </c>
       <c r="B163" s="1" t="s">
         <v>5</v>
@@ -4913,7 +4966,7 @@
     </row>
     <row r="164" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A164" s="1" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="B164" s="1" t="s">
         <v>5</v>
@@ -4927,7 +4980,7 @@
     </row>
     <row r="165" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A165" s="1" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="B165" s="1" t="s">
         <v>12</v>
@@ -4941,7 +4994,7 @@
     </row>
     <row r="166" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A166" s="1" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="B166" s="1" t="s">
         <v>12</v>
@@ -4955,7 +5008,7 @@
     </row>
     <row r="167" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A167" s="1" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="B167" s="1" t="s">
         <v>5</v>
@@ -4969,7 +5022,7 @@
     </row>
     <row r="168" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A168" s="1" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="B168" s="1" t="s">
         <v>5</v>
@@ -4983,7 +5036,7 @@
     </row>
     <row r="169" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A169" s="1" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="B169" s="1" t="s">
         <v>16</v>
@@ -4997,7 +5050,7 @@
     </row>
     <row r="170" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A170" s="1" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="B170" s="1" t="s">
         <v>16</v>
@@ -5011,7 +5064,7 @@
     </row>
     <row r="171" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A171" s="1" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="B171" s="1" t="s">
         <v>5</v>
@@ -5025,7 +5078,7 @@
     </row>
     <row r="172" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A172" s="1" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="B172" s="1" t="s">
         <v>5</v>
@@ -5039,7 +5092,7 @@
     </row>
     <row r="173" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A173" s="1" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="B173" s="1" t="s">
         <v>5</v>
@@ -5053,7 +5106,7 @@
     </row>
     <row r="175" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A175" s="0" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="B175" s="1" t="s">
         <v>5</v>
@@ -5070,7 +5123,7 @@
     </row>
     <row r="176" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A176" s="0" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="B176" s="1" t="s">
         <v>5</v>
@@ -5084,7 +5137,7 @@
     </row>
     <row r="177" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A177" s="1" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="B177" s="1" t="s">
         <v>5</v>
@@ -5097,8 +5150,8 @@
       </c>
     </row>
     <row r="178" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A178" s="7" t="s">
-        <v>173</v>
+      <c r="A178" s="1" t="s">
+        <v>175</v>
       </c>
       <c r="B178" s="1" t="s">
         <v>5</v>
@@ -5112,7 +5165,7 @@
     </row>
     <row r="179" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A179" s="1" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="B179" s="1" t="s">
         <v>5</v>
@@ -5126,7 +5179,7 @@
     </row>
     <row r="180" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A180" s="1" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="B180" s="1" t="s">
         <v>5</v>
@@ -5140,7 +5193,7 @@
     </row>
     <row r="181" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A181" s="1" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="B181" s="1" t="s">
         <v>5</v>
@@ -5154,7 +5207,7 @@
     </row>
     <row r="182" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A182" s="1" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="B182" s="1" t="s">
         <v>5</v>
@@ -5168,7 +5221,7 @@
     </row>
     <row r="184" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A184" s="1" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="B184" s="1" t="s">
         <v>5</v>
@@ -5184,8 +5237,8 @@
       </c>
     </row>
     <row r="185" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A185" s="7" t="s">
-        <v>179</v>
+      <c r="A185" s="1" t="s">
+        <v>181</v>
       </c>
       <c r="B185" s="1" t="s">
         <v>5</v>
@@ -5199,7 +5252,7 @@
     </row>
     <row r="186" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A186" s="1" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="B186" s="1" t="s">
         <v>5</v>
@@ -5213,7 +5266,7 @@
     </row>
     <row r="187" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A187" s="1" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="B187" s="1" t="s">
         <v>12</v>
@@ -5226,8 +5279,8 @@
       </c>
     </row>
     <row r="188" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A188" s="7" t="s">
-        <v>181</v>
+      <c r="A188" s="1" t="s">
+        <v>183</v>
       </c>
       <c r="B188" s="1" t="s">
         <v>12</v>
@@ -5241,7 +5294,7 @@
     </row>
     <row r="189" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A189" s="1" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="B189" s="1" t="s">
         <v>5</v>
@@ -5255,7 +5308,7 @@
     </row>
     <row r="190" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A190" s="0" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="B190" s="1" t="s">
         <v>5</v>
@@ -5269,7 +5322,7 @@
     </row>
     <row r="191" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A191" s="1" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="B191" s="1" t="s">
         <v>16</v>
@@ -5283,7 +5336,7 @@
     </row>
     <row r="192" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A192" s="1" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="B192" s="1" t="s">
         <v>16</v>
@@ -5296,8 +5349,8 @@
       </c>
     </row>
     <row r="193" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A193" s="7" t="s">
-        <v>185</v>
+      <c r="A193" s="1" t="s">
+        <v>187</v>
       </c>
       <c r="B193" s="1" t="s">
         <v>5</v>
@@ -5311,7 +5364,7 @@
     </row>
     <row r="194" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A194" s="1" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="B194" s="1" t="s">
         <v>5</v>
@@ -5325,7 +5378,7 @@
     </row>
     <row r="195" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A195" s="1" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="B195" s="1" t="s">
         <v>5</v>
@@ -5339,7 +5392,7 @@
     </row>
     <row r="197" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A197" s="1" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="B197" s="1" t="s">
         <v>5</v>
@@ -5356,7 +5409,7 @@
     </row>
     <row r="198" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A198" s="1" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="B198" s="1" t="s">
         <v>5</v>
@@ -5370,7 +5423,7 @@
     </row>
     <row r="199" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A199" s="1" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="B199" s="1" t="s">
         <v>5</v>
@@ -5384,7 +5437,7 @@
     </row>
     <row r="200" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A200" s="1" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="B200" s="1" t="s">
         <v>12</v>
@@ -5398,7 +5451,7 @@
     </row>
     <row r="201" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A201" s="1" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="B201" s="1" t="s">
         <v>12</v>
@@ -5411,8 +5464,8 @@
       </c>
     </row>
     <row r="202" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A202" s="7" t="s">
-        <v>192</v>
+      <c r="A202" s="1" t="s">
+        <v>194</v>
       </c>
       <c r="B202" s="1" t="s">
         <v>5</v>
@@ -5426,7 +5479,7 @@
     </row>
     <row r="203" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A203" s="0" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="B203" s="1" t="s">
         <v>5</v>
@@ -5440,7 +5493,7 @@
     </row>
     <row r="204" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A204" s="0" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="B204" s="1" t="s">
         <v>5</v>
@@ -5454,7 +5507,7 @@
     </row>
     <row r="205" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A205" s="1" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="B205" s="1" t="s">
         <v>5</v>
@@ -5468,7 +5521,7 @@
     </row>
     <row r="206" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A206" s="1" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="B206" s="1" t="s">
         <v>5</v>
@@ -5482,7 +5535,7 @@
     </row>
     <row r="208" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A208" s="0" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="B208" s="1" t="s">
         <v>5</v>
@@ -5498,8 +5551,8 @@
       </c>
     </row>
     <row r="209" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A209" s="7" t="s">
-        <v>198</v>
+      <c r="A209" s="1" t="s">
+        <v>200</v>
       </c>
       <c r="B209" s="1" t="s">
         <v>5</v>
@@ -5513,7 +5566,7 @@
     </row>
     <row r="210" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A210" s="1" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="B210" s="1" t="s">
         <v>5</v>
@@ -5527,7 +5580,7 @@
     </row>
     <row r="211" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A211" s="1" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="B211" s="1" t="s">
         <v>5</v>
@@ -5541,7 +5594,7 @@
     </row>
     <row r="212" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A212" s="1" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="B212" s="1" t="s">
         <v>5</v>
@@ -5555,7 +5608,7 @@
     </row>
     <row r="213" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A213" s="1" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="B213" s="1" t="s">
         <v>16</v>
@@ -5569,7 +5622,7 @@
     </row>
     <row r="214" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A214" s="1" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="B214" s="1" t="s">
         <v>16</v>
@@ -5583,7 +5636,7 @@
     </row>
     <row r="215" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A215" s="1" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="B215" s="1" t="s">
         <v>5</v>
@@ -5597,7 +5650,7 @@
     </row>
     <row r="216" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A216" s="1" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="B216" s="1" t="s">
         <v>5</v>
@@ -5611,7 +5664,7 @@
     </row>
     <row r="217" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A217" s="1" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="B217" s="1" t="s">
         <v>5</v>
@@ -5625,7 +5678,7 @@
     </row>
     <row r="219" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A219" s="0" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="B219" s="1" t="s">
         <v>5</v>
@@ -5642,7 +5695,7 @@
     </row>
     <row r="220" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A220" s="0" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="B220" s="1" t="s">
         <v>5</v>
@@ -5656,7 +5709,7 @@
     </row>
     <row r="221" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A221" s="1" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="B221" s="1" t="s">
         <v>5</v>
@@ -5670,7 +5723,7 @@
     </row>
     <row r="222" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A222" s="1" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="B222" s="1" t="s">
         <v>5</v>
@@ -5684,7 +5737,7 @@
     </row>
     <row r="223" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A223" s="1" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="B223" s="1" t="s">
         <v>5</v>
@@ -5698,7 +5751,7 @@
     </row>
     <row r="224" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A224" s="1" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="B224" s="1" t="s">
         <v>5</v>
@@ -5712,7 +5765,7 @@
     </row>
     <row r="225" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A225" s="1" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="B225" s="1" t="s">
         <v>5</v>
@@ -5726,7 +5779,7 @@
     </row>
     <row r="226" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A226" s="1" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="B226" s="1" t="s">
         <v>5</v>
@@ -5740,7 +5793,7 @@
     </row>
     <row r="228" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A228" s="1" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="B228" s="1" t="s">
         <v>5</v>
@@ -5757,7 +5810,7 @@
     </row>
     <row r="229" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A229" s="1" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="B229" s="1" t="s">
         <v>5</v>
@@ -5771,7 +5824,7 @@
     </row>
     <row r="230" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A230" s="1" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="B230" s="1" t="s">
         <v>5</v>
@@ -5785,7 +5838,7 @@
     </row>
     <row r="231" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A231" s="1" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="B231" s="1" t="s">
         <v>12</v>
@@ -5799,7 +5852,7 @@
     </row>
     <row r="232" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A232" s="1" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="B232" s="1" t="s">
         <v>12</v>
@@ -5813,7 +5866,7 @@
     </row>
     <row r="233" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A233" s="1" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="B233" s="1" t="s">
         <v>5</v>
@@ -5827,7 +5880,7 @@
     </row>
     <row r="234" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A234" s="0" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="B234" s="1" t="s">
         <v>5</v>
@@ -5841,7 +5894,7 @@
     </row>
     <row r="235" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A235" s="1" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="B235" s="1" t="s">
         <v>5</v>
@@ -5855,7 +5908,7 @@
     </row>
     <row r="236" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A236" s="1" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="B236" s="1" t="s">
         <v>5</v>
@@ -5869,7 +5922,7 @@
     </row>
     <row r="237" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A237" s="1" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="B237" s="1" t="s">
         <v>5</v>

</xml_diff>